<commit_message>
Updated code for data processing
</commit_message>
<xml_diff>
--- a/data/First_round_results/First Plate 260220 (Rep 2 of 6).xlsx
+++ b/data/First_round_results/First Plate 260220 (Rep 2 of 6).xlsx
@@ -8,20 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOL428\Documents\GitHub\SynbioML\data\First_round_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30D18F9-D855-4D58-B0BC-3B9996825928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EA2CEF-E6F8-4216-806E-B21A734DB350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BFBB8FCE-10C2-4D1D-812E-8177E01F1C3E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OD" sheetId="1" r:id="rId1"/>
-    <sheet name="GFP" sheetId="3" r:id="rId2"/>
-    <sheet name="ODGFP" sheetId="2" r:id="rId3"/>
+    <sheet name="GFP" sheetId="2" r:id="rId2"/>
+    <sheet name="ODGFP" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -394,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -403,9 +400,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -721,10 +715,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58F984F-4914-4C3B-98A2-2322FA614F2F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection sqref="A1:CS50"/>
     </sheetView>
   </sheetViews>
@@ -1318,7 +1312,7 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>1.2766203703703703E-2</v>
+        <v>1.27662037037037E-2</v>
       </c>
       <c r="B3" s="3">
         <v>0.16200000000000001</v>
@@ -1611,7 +1605,7 @@
     </row>
     <row r="4" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>1.9710648148148147E-2</v>
+        <v>1.9710648148148151E-2</v>
       </c>
       <c r="B4" s="3">
         <v>0.17699999999999999</v>
@@ -3369,7 +3363,7 @@
     </row>
     <row r="10" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>6.1377314814814815E-2</v>
+        <v>6.1377314814814822E-2</v>
       </c>
       <c r="B10" s="3">
         <v>0.27200000000000002</v>
@@ -3955,7 +3949,7 @@
     </row>
     <row r="12" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>7.5266203703703696E-2</v>
+        <v>7.526620370370371E-2</v>
       </c>
       <c r="B12" s="3">
         <v>0.29899999999999999</v>
@@ -5127,7 +5121,7 @@
     </row>
     <row r="16" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
-        <v>0.10304398148148149</v>
+        <v>0.1030439814814815</v>
       </c>
       <c r="B16" s="3">
         <v>0.33300000000000002</v>
@@ -5420,7 +5414,7 @@
     </row>
     <row r="17" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>0.10998842592592593</v>
+        <v>0.10998842592592591</v>
       </c>
       <c r="B17" s="3">
         <v>0.34</v>
@@ -5713,7 +5707,7 @@
     </row>
     <row r="18" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
-        <v>0.11693287037037037</v>
+        <v>0.1169328703703704</v>
       </c>
       <c r="B18" s="3">
         <v>0.34899999999999998</v>
@@ -6006,7 +6000,7 @@
     </row>
     <row r="19" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
-        <v>0.12387731481481483</v>
+        <v>0.1238773148148148</v>
       </c>
       <c r="B19" s="3">
         <v>0.35399999999999998</v>
@@ -6299,7 +6293,7 @@
     </row>
     <row r="20" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
-        <v>0.13082175925925926</v>
+        <v>0.13082175925925929</v>
       </c>
       <c r="B20" s="3">
         <v>0.35899999999999999</v>
@@ -6885,7 +6879,7 @@
     </row>
     <row r="22" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <v>0.14471064814814816</v>
+        <v>0.14471064814814821</v>
       </c>
       <c r="B22" s="3">
         <v>0.373</v>
@@ -7471,7 +7465,7 @@
     </row>
     <row r="24" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
-        <v>0.15859953703703702</v>
+        <v>0.158599537037037</v>
       </c>
       <c r="B24" s="3">
         <v>0.38600000000000001</v>
@@ -8057,7 +8051,7 @@
     </row>
     <row r="26" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
-        <v>0.17248842592592592</v>
+        <v>0.17248842592592589</v>
       </c>
       <c r="B26" s="3">
         <v>0.39700000000000002</v>
@@ -8350,7 +8344,7 @@
     </row>
     <row r="27" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
-        <v>0.17943287037037037</v>
+        <v>0.1794328703703704</v>
       </c>
       <c r="B27" s="3">
         <v>0.40699999999999997</v>
@@ -8643,7 +8637,7 @@
     </row>
     <row r="28" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
-        <v>0.18637731481481482</v>
+        <v>0.18637731481481479</v>
       </c>
       <c r="B28" s="3">
         <v>0.41199999999999998</v>
@@ -8936,7 +8930,7 @@
     </row>
     <row r="29" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
-        <v>0.19332175925925923</v>
+        <v>0.19332175925925929</v>
       </c>
       <c r="B29" s="3">
         <v>0.41799999999999998</v>
@@ -9522,7 +9516,7 @@
     </row>
     <row r="31" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
-        <v>0.20721064814814816</v>
+        <v>0.20721064814814821</v>
       </c>
       <c r="B31" s="3">
         <v>0.432</v>
@@ -9815,7 +9809,7 @@
     </row>
     <row r="32" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
-        <v>0.21415509259259258</v>
+        <v>0.21415509259259261</v>
       </c>
       <c r="B32" s="3">
         <v>0.442</v>
@@ -10108,7 +10102,7 @@
     </row>
     <row r="33" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
-        <v>0.22109953703703702</v>
+        <v>0.221099537037037</v>
       </c>
       <c r="B33" s="3">
         <v>0.45200000000000001</v>
@@ -10694,7 +10688,7 @@
     </row>
     <row r="35" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
-        <v>0.23498842592592592</v>
+        <v>0.23498842592592589</v>
       </c>
       <c r="B35" s="3">
         <v>0.45400000000000001</v>
@@ -10987,7 +10981,7 @@
     </row>
     <row r="36" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
-        <v>0.24193287037037037</v>
+        <v>0.2419328703703704</v>
       </c>
       <c r="B36" s="3">
         <v>0.45100000000000001</v>
@@ -11280,7 +11274,7 @@
     </row>
     <row r="37" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
-        <v>0.24887731481481482</v>
+        <v>0.24887731481481479</v>
       </c>
       <c r="B37" s="3">
         <v>0.46400000000000002</v>
@@ -11573,7 +11567,7 @@
     </row>
     <row r="38" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
-        <v>0.25582175925925926</v>
+        <v>0.25582175925925932</v>
       </c>
       <c r="B38" s="3">
         <v>0.45700000000000002</v>
@@ -12159,7 +12153,7 @@
     </row>
     <row r="40" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
-        <v>0.26971064814814816</v>
+        <v>0.26971064814814821</v>
       </c>
       <c r="B40" s="3">
         <v>0.45800000000000002</v>
@@ -12745,7 +12739,7 @@
     </row>
     <row r="42" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
-        <v>0.28359953703703705</v>
+        <v>0.28359953703703711</v>
       </c>
       <c r="B42" s="3">
         <v>0.46600000000000003</v>
@@ -13624,7 +13618,7 @@
     </row>
     <row r="45" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
-        <v>0.30443287037037037</v>
+        <v>0.30443287037037042</v>
       </c>
       <c r="B45" s="3">
         <v>0.46600000000000003</v>
@@ -13917,7 +13911,7 @@
     </row>
     <row r="46" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
-        <v>0.31137731481481484</v>
+        <v>0.31137731481481479</v>
       </c>
       <c r="B46" s="3">
         <v>0.46899999999999997</v>
@@ -14210,7 +14204,7 @@
     </row>
     <row r="47" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
-        <v>0.31832175925925926</v>
+        <v>0.31832175925925932</v>
       </c>
       <c r="B47" s="3">
         <v>0.47199999999999998</v>
@@ -14796,7 +14790,7 @@
     </row>
     <row r="49" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
-        <v>0.33221064814814816</v>
+        <v>0.33221064814814821</v>
       </c>
       <c r="B49" s="3">
         <v>0.46500000000000002</v>
@@ -15394,12 +15388,12 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="156" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="156" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289FFCC8-6B62-4E1B-8ABE-FE0DA500FA1A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CS50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15703,7 +15697,7 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>6.6550925925925935E-3</v>
+        <v>6.6550925925925927E-3</v>
       </c>
       <c r="B2" s="3">
         <v>48</v>
@@ -15996,7 +15990,7 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>1.3599537037037037E-2</v>
+        <v>1.359953703703704E-2</v>
       </c>
       <c r="B3" s="3">
         <v>58</v>
@@ -16582,7 +16576,7 @@
     </row>
     <row r="5" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>2.7488425925925927E-2</v>
+        <v>2.748842592592593E-2</v>
       </c>
       <c r="B5" s="3">
         <v>57</v>
@@ -17461,7 +17455,7 @@
     </row>
     <row r="8" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>4.8321759259259266E-2</v>
+        <v>4.8321759259259259E-2</v>
       </c>
       <c r="B8" s="3">
         <v>58</v>
@@ -17754,7 +17748,7 @@
     </row>
     <row r="9" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>5.5266203703703699E-2</v>
+        <v>5.5266203703703713E-2</v>
       </c>
       <c r="B9" s="3">
         <v>63</v>
@@ -18340,7 +18334,7 @@
     </row>
     <row r="11" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>6.9155092592592601E-2</v>
+        <v>6.9155092592592587E-2</v>
       </c>
       <c r="B11" s="3">
         <v>77</v>
@@ -19805,7 +19799,7 @@
     </row>
     <row r="16" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
-        <v>0.10387731481481481</v>
+        <v>0.1038773148148148</v>
       </c>
       <c r="B16" s="3">
         <v>115</v>
@@ -20098,7 +20092,7 @@
     </row>
     <row r="17" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>0.11082175925925926</v>
+        <v>0.1108217592592593</v>
       </c>
       <c r="B17" s="3">
         <v>130</v>
@@ -20684,7 +20678,7 @@
     </row>
     <row r="19" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
-        <v>0.12471064814814814</v>
+        <v>0.1247106481481482</v>
       </c>
       <c r="B19" s="3">
         <v>161</v>
@@ -21270,7 +21264,7 @@
     </row>
     <row r="21" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
-        <v>0.13859953703703703</v>
+        <v>0.13859953703703701</v>
       </c>
       <c r="B21" s="3">
         <v>176</v>
@@ -21563,7 +21557,7 @@
     </row>
     <row r="22" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <v>0.14554398148148148</v>
+        <v>0.14554398148148151</v>
       </c>
       <c r="B22" s="3">
         <v>202</v>
@@ -21856,7 +21850,7 @@
     </row>
     <row r="23" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
-        <v>0.15248842592592593</v>
+        <v>0.1524884259259259</v>
       </c>
       <c r="B23" s="3">
         <v>226</v>
@@ -22149,7 +22143,7 @@
     </row>
     <row r="24" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
-        <v>0.15943287037037038</v>
+        <v>0.15943287037037041</v>
       </c>
       <c r="B24" s="3">
         <v>239</v>
@@ -22735,7 +22729,7 @@
     </row>
     <row r="26" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
-        <v>0.17332175925925927</v>
+        <v>0.1733217592592593</v>
       </c>
       <c r="B26" s="3">
         <v>277</v>
@@ -23028,7 +23022,7 @@
     </row>
     <row r="27" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
-        <v>0.18026620370370372</v>
+        <v>0.18026620370370369</v>
       </c>
       <c r="B27" s="3">
         <v>291</v>
@@ -23321,7 +23315,7 @@
     </row>
     <row r="28" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
-        <v>0.18721064814814814</v>
+        <v>0.18721064814814811</v>
       </c>
       <c r="B28" s="3">
         <v>323</v>
@@ -23907,7 +23901,7 @@
     </row>
     <row r="30" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
-        <v>0.20109953703703706</v>
+        <v>0.20109953703703701</v>
       </c>
       <c r="B30" s="3">
         <v>335</v>
@@ -24200,7 +24194,7 @@
     </row>
     <row r="31" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
-        <v>0.20804398148148148</v>
+        <v>0.20804398148148151</v>
       </c>
       <c r="B31" s="3">
         <v>370</v>
@@ -24493,7 +24487,7 @@
     </row>
     <row r="32" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
-        <v>0.21498842592592593</v>
+        <v>0.2149884259259259</v>
       </c>
       <c r="B32" s="3">
         <v>381</v>
@@ -24786,7 +24780,7 @@
     </row>
     <row r="33" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
-        <v>0.22193287037037038</v>
+        <v>0.22193287037037041</v>
       </c>
       <c r="B33" s="3">
         <v>416</v>
@@ -25372,7 +25366,7 @@
     </row>
     <row r="35" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
-        <v>0.23582175925925927</v>
+        <v>0.2358217592592593</v>
       </c>
       <c r="B35" s="3">
         <v>436</v>
@@ -25665,7 +25659,7 @@
     </row>
     <row r="36" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
-        <v>0.24276620370370372</v>
+        <v>0.24276620370370369</v>
       </c>
       <c r="B36" s="3">
         <v>467</v>
@@ -25958,7 +25952,7 @@
     </row>
     <row r="37" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
-        <v>0.24971064814814814</v>
+        <v>0.24971064814814811</v>
       </c>
       <c r="B37" s="3">
         <v>483</v>
@@ -26544,7 +26538,7 @@
     </row>
     <row r="39" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
-        <v>0.26359953703703703</v>
+        <v>0.26359953703703698</v>
       </c>
       <c r="B39" s="3">
         <v>505</v>
@@ -26837,7 +26831,7 @@
     </row>
     <row r="40" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
-        <v>0.27054398148148145</v>
+        <v>0.27054398148148151</v>
       </c>
       <c r="B40" s="3">
         <v>533</v>
@@ -27130,7 +27124,7 @@
     </row>
     <row r="41" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
-        <v>0.27748842592592593</v>
+        <v>0.27748842592592587</v>
       </c>
       <c r="B41" s="3">
         <v>534</v>
@@ -27423,7 +27417,7 @@
     </row>
     <row r="42" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
-        <v>0.28443287037037041</v>
+        <v>0.28443287037037029</v>
       </c>
       <c r="B42" s="3">
         <v>547</v>
@@ -28009,7 +28003,7 @@
     </row>
     <row r="44" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
-        <v>0.29832175925925924</v>
+        <v>0.29832175925925919</v>
       </c>
       <c r="B44" s="3">
         <v>564</v>
@@ -28595,7 +28589,7 @@
     </row>
     <row r="46" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
-        <v>0.31221064814814814</v>
+        <v>0.31221064814814808</v>
       </c>
       <c r="B46" s="3">
         <v>581</v>
@@ -29181,7 +29175,7 @@
     </row>
     <row r="48" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
-        <v>0.32609953703703703</v>
+        <v>0.32609953703703698</v>
       </c>
       <c r="B48" s="3">
         <v>620</v>
@@ -29474,7 +29468,7 @@
     </row>
     <row r="49" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
-        <v>0.33304398148148145</v>
+        <v>0.33304398148148151</v>
       </c>
       <c r="B49" s="3">
         <v>615</v>
@@ -30064,11 +30058,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7546449-E5B9-47B0-BC61-E9C5925153EB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CL50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30349,7 +30343,7 @@
       </c>
     </row>
     <row r="2" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>0</v>
       </c>
       <c r="B2" s="3">
@@ -30710,7 +30704,7 @@
       </c>
     </row>
     <row r="3" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>10</v>
       </c>
       <c r="B3" s="3">
@@ -31071,7 +31065,7 @@
       </c>
     </row>
     <row r="4" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>20</v>
       </c>
       <c r="B4" s="3">
@@ -31432,7 +31426,7 @@
       </c>
     </row>
     <row r="5" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>30</v>
       </c>
       <c r="B5" s="3">
@@ -31793,7 +31787,7 @@
       </c>
     </row>
     <row r="6" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>40</v>
       </c>
       <c r="B6" s="3">
@@ -32154,7 +32148,7 @@
       </c>
     </row>
     <row r="7" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>50</v>
       </c>
       <c r="B7" s="3">
@@ -32515,7 +32509,7 @@
       </c>
     </row>
     <row r="8" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>60</v>
       </c>
       <c r="B8" s="3">
@@ -32876,7 +32870,7 @@
       </c>
     </row>
     <row r="9" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>70</v>
       </c>
       <c r="B9" s="3">
@@ -33237,7 +33231,7 @@
       </c>
     </row>
     <row r="10" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>80</v>
       </c>
       <c r="B10" s="3">
@@ -33598,7 +33592,7 @@
       </c>
     </row>
     <row r="11" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>90</v>
       </c>
       <c r="B11" s="3">
@@ -33959,7 +33953,7 @@
       </c>
     </row>
     <row r="12" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>100</v>
       </c>
       <c r="B12" s="3">
@@ -34320,7 +34314,7 @@
       </c>
     </row>
     <row r="13" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>110</v>
       </c>
       <c r="B13" s="3">
@@ -34681,7 +34675,7 @@
       </c>
     </row>
     <row r="14" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>120</v>
       </c>
       <c r="B14" s="3">
@@ -35042,7 +35036,7 @@
       </c>
     </row>
     <row r="15" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>130</v>
       </c>
       <c r="B15" s="3">
@@ -35403,7 +35397,7 @@
       </c>
     </row>
     <row r="16" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>140</v>
       </c>
       <c r="B16" s="3">
@@ -35764,7 +35758,7 @@
       </c>
     </row>
     <row r="17" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>150</v>
       </c>
       <c r="B17" s="3">
@@ -36125,7 +36119,7 @@
       </c>
     </row>
     <row r="18" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>160</v>
       </c>
       <c r="B18" s="3">
@@ -36486,7 +36480,7 @@
       </c>
     </row>
     <row r="19" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>170</v>
       </c>
       <c r="B19" s="3">
@@ -36847,7 +36841,7 @@
       </c>
     </row>
     <row r="20" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>180</v>
       </c>
       <c r="B20" s="3">
@@ -37208,7 +37202,7 @@
       </c>
     </row>
     <row r="21" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>190</v>
       </c>
       <c r="B21" s="3">
@@ -37569,7 +37563,7 @@
       </c>
     </row>
     <row r="22" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>200</v>
       </c>
       <c r="B22" s="3">
@@ -37930,7 +37924,7 @@
       </c>
     </row>
     <row r="23" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>210</v>
       </c>
       <c r="B23" s="3">
@@ -38291,7 +38285,7 @@
       </c>
     </row>
     <row r="24" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>220</v>
       </c>
       <c r="B24" s="3">
@@ -38652,7 +38646,7 @@
       </c>
     </row>
     <row r="25" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>230</v>
       </c>
       <c r="B25" s="3">
@@ -39013,7 +39007,7 @@
       </c>
     </row>
     <row r="26" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>240</v>
       </c>
       <c r="B26" s="3">
@@ -39374,7 +39368,7 @@
       </c>
     </row>
     <row r="27" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>250</v>
       </c>
       <c r="B27" s="3">
@@ -39735,7 +39729,7 @@
       </c>
     </row>
     <row r="28" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>260</v>
       </c>
       <c r="B28" s="3">
@@ -40096,7 +40090,7 @@
       </c>
     </row>
     <row r="29" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>270</v>
       </c>
       <c r="B29" s="3">
@@ -40457,7 +40451,7 @@
       </c>
     </row>
     <row r="30" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>280</v>
       </c>
       <c r="B30" s="3">
@@ -40818,7 +40812,7 @@
       </c>
     </row>
     <row r="31" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>290</v>
       </c>
       <c r="B31" s="3">
@@ -41179,7 +41173,7 @@
       </c>
     </row>
     <row r="32" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <v>300</v>
       </c>
       <c r="B32" s="3">
@@ -41540,7 +41534,7 @@
       </c>
     </row>
     <row r="33" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>310</v>
       </c>
       <c r="B33" s="3">
@@ -41901,7 +41895,7 @@
       </c>
     </row>
     <row r="34" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>320</v>
       </c>
       <c r="B34" s="3">
@@ -42262,7 +42256,7 @@
       </c>
     </row>
     <row r="35" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>330</v>
       </c>
       <c r="B35" s="3">
@@ -42623,7 +42617,7 @@
       </c>
     </row>
     <row r="36" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>340</v>
       </c>
       <c r="B36" s="3">
@@ -42984,7 +42978,7 @@
       </c>
     </row>
     <row r="37" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>350</v>
       </c>
       <c r="B37" s="3">
@@ -43345,7 +43339,7 @@
       </c>
     </row>
     <row r="38" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>360</v>
       </c>
       <c r="B38" s="3">
@@ -43706,7 +43700,7 @@
       </c>
     </row>
     <row r="39" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A39" s="4">
+      <c r="A39" s="3">
         <v>370</v>
       </c>
       <c r="B39" s="3">
@@ -44067,7 +44061,7 @@
       </c>
     </row>
     <row r="40" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>380</v>
       </c>
       <c r="B40" s="3">
@@ -44428,7 +44422,7 @@
       </c>
     </row>
     <row r="41" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A41" s="4">
+      <c r="A41" s="3">
         <v>390</v>
       </c>
       <c r="B41" s="3">
@@ -44789,7 +44783,7 @@
       </c>
     </row>
     <row r="42" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A42" s="4">
+      <c r="A42" s="3">
         <v>400</v>
       </c>
       <c r="B42" s="3">
@@ -45150,7 +45144,7 @@
       </c>
     </row>
     <row r="43" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A43" s="4">
+      <c r="A43" s="3">
         <v>410</v>
       </c>
       <c r="B43" s="3">
@@ -45511,7 +45505,7 @@
       </c>
     </row>
     <row r="44" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A44" s="4">
+      <c r="A44" s="3">
         <v>420</v>
       </c>
       <c r="B44" s="3">
@@ -45872,7 +45866,7 @@
       </c>
     </row>
     <row r="45" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A45" s="4">
+      <c r="A45" s="3">
         <v>430</v>
       </c>
       <c r="B45" s="3">
@@ -46233,7 +46227,7 @@
       </c>
     </row>
     <row r="46" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A46" s="4">
+      <c r="A46" s="3">
         <v>440</v>
       </c>
       <c r="B46" s="3">
@@ -46594,7 +46588,7 @@
       </c>
     </row>
     <row r="47" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A47" s="4">
+      <c r="A47" s="3">
         <v>450</v>
       </c>
       <c r="B47" s="3">
@@ -46955,7 +46949,7 @@
       </c>
     </row>
     <row r="48" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A48" s="4">
+      <c r="A48" s="3">
         <v>460</v>
       </c>
       <c r="B48" s="3">
@@ -47316,7 +47310,7 @@
       </c>
     </row>
     <row r="49" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A49" s="4">
+      <c r="A49" s="3">
         <v>470</v>
       </c>
       <c r="B49" s="3">
@@ -47677,7 +47671,7 @@
       </c>
     </row>
     <row r="50" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="A50" s="4">
+      <c r="A50" s="3">
         <v>480</v>
       </c>
       <c r="B50" s="3">
@@ -48039,6 +48033,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>